<commit_message>
Language fixes in scenarios
</commit_message>
<xml_diff>
--- a/scenarios-v6-v7/2023-10-28-DeleteModifyScenarios.xlsx
+++ b/scenarios-v6-v7/2023-10-28-DeleteModifyScenarios.xlsx
@@ -140,33 +140,6 @@
     <t>A sends IIA GET with B.iia_id (remote), receives in response B1 (A.iia_id, B.iia_id, B1.hash2)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve">A sends IIA GET with B.iia_id (remote), receives in response B0 (A.iia_id, B.iia_id, B0.hash0)
-A recognizes, that B </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="2"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t>reverted back</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve"> to revision B0</t>
-    </r>
-  </si>
-  <si>
     <t>Final state</t>
   </si>
   <si>
@@ -284,144 +257,6 @@
       <t xml:space="preserve"> request with A.iia_id (local), receives in response (A.iia_id, A1.hash1)
 mapped identifiers: B.iia_id (local), A.iia_id (remote)
 last known hashes: A1.hash1, B1.hash1
-approval hashes: A1.hash1, B0.hash0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve">A changed their mind - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="2"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve">removes </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve">A1 and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="2"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t>reverts back</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve"> to A0
-mapped identifiers: B.iia_id (local), A.iia_id (remote)
-last known hashes: A0.hash0, B1.hash1
-approval hashes: A1.hash1, B0.hash0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve">B sends IIA GET, receives in response A0 (A.iia_id, B.iia_id, A0.hash0)
-B recognized that A </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="2"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t>reverted back</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve"> to revision A0 (A0.hash0)
-B </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="2"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve">removes </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve">revision B1 and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="2"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t>reverts back</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve"> to B0
-mapped identifiers: B.iia_id (local), A.iia_id (remote)
-last known hashes: B0.hash0, A0.hash0
-approval hashes: B0.hash0, A1.hash1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve">A sends IIA GET with B.iia_id (remote), receives in response B0 (A.iia_id, B.iia_id, B0.hash0)
-A recognized, that B </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="2"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t>reverted back</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve"> to revision B0
-mapped identifiers: B.iia_id (local), A.iia_id (remote)
-last known hashes: A0.hash0, B0.hash0
 approval hashes: A1.hash1, B0.hash0</t>
     </r>
   </si>
@@ -1382,142 +1217,6 @@
     <t>A sends IIA GET with B.iia_id (remote), receives in response B1 (A.iia_id, B.iia_id, B1.iia-hash2)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve">A does not like changes presented in B1 and wants to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="2"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t>revert back</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve"> to A0
-A </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="2"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t>removes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve"> A1
-mapped identifiers: A.iia_id (local), B.iia_id (remote)
-last known hashes: A0.iia-hash0, B0.iia-hash0
-approval hashes: A0.iia-hash0, B0.iia-hash0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve">B sends IIA GET with A.iia_id (remote), receives in response A0 (A.iia_id, B.iia_id, A0.iia-hash0)
-B recognizes, that A </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="2"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t>reverted back</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve"> to revision A0 (A0.iia-hash0)
-B </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="2"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t>removes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve"> revision B1 and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="2"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t>reverts back</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve"> to revision B0
-mapped identifiers: B.iia_id (local), A.iia_id (remote)
-last known hashes: B0.iia-hash0, A0.iia-hash0
-approval hashes: B0.iia-hash0, A0.iia-hash0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve">A sends IIA GET with B.iia_id (remote), receives in response B0 (A.iia_id, B.iia_id, B0.iia-hash0)
-A recognizes, that B </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="2"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t>reverted back</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve"> to revision B0</t>
-    </r>
-  </si>
-  <si>
     <t>IIA - revision A0 (mutually approved)  
 mapped identifiers: A.iia_id (local), B.iia_id (remote) 
 last known hashes: A0.iia-hash0, B0.iia-hash0
@@ -1528,105 +1227,6 @@
 mapped identifiers: B.iia_id (local), A.iia_id (remote)
 last known hashes: B0.iia-hash0, A0.iia-hash0 
 approval hashes: B0.iia-hash0, A0.iia-hash0</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A does not like changes presented in B1 and wants to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="2"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t>revert back</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve"> to A0
-A </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="2"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve">removes </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t>A1
-mapped identifiers: A.iia_id (local), B.iia_id (remote)
-last known hashes: A0.hash0, B0.hash0
-approval hashes: A0.hash0, B0.hash0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">B sends IIA GET with A.iia_id (remote), receives in response A0 (A.iia_id, B.iia_id, A0.hash0)
-B recognizes, that A </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="2"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t>reverted back</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve"> to revision A0 (A0.hash0)
-B </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="2"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve">removes </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve">revision B1 and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="2"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t>reverts back</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Czcionka tekstu podstawowego"/>
-      </rPr>
-      <t xml:space="preserve"> to revision B0
-mapped identifiers: B.iia_id (local), A.iia_id (remote)
-last known hashes: B0.hash0, A0.hash0
-approval hashes: B0.hash0, A0.hash0</t>
-    </r>
   </si>
   <si>
     <r>
@@ -2388,6 +1988,371 @@
         <rFont val="Czcionka tekstu podstawowego"/>
       </rPr>
       <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A does not like changes presented in B1 and wants to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="2"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">revert </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">to A0
+A </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="2"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t>removes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve"> A1
+mapped identifiers: A.iia_id (local), B.iia_id (remote)
+last known hashes: A0.iia-hash0, B0.iia-hash0
+approval hashes: A0.iia-hash0, B0.iia-hash0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B sends IIA GET with A.iia_id (remote), receives in response A0 (A.iia_id, B.iia_id, A0.iia-hash0)
+B recognizes, that A </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="2"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">reverted </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">to revision A0 (A0.iia-hash0)
+B </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="2"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t>removes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve"> revision B1 and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="2"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">reverts </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve"> to revision B0
+mapped identifiers: B.iia_id (local), A.iia_id (remote)
+last known hashes: B0.iia-hash0, A0.iia-hash0
+approval hashes: B0.iia-hash0, A0.iia-hash0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A sends IIA GET with B.iia_id (remote), receives in response B0 (A.iia_id, B.iia_id, B0.iia-hash0)
+A recognizes, that B </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="2"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">reverted </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t>to revision B0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A does not like changes presented in B1 and wants to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="2"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t>revert</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve"> to A0
+A </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="2"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">removes </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t>A1
+mapped identifiers: A.iia_id (local), B.iia_id (remote)
+last known hashes: A0.hash0, B0.hash0
+approval hashes: A0.hash0, B0.hash0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B sends IIA GET with A.iia_id (remote), receives in response A0 (A.iia_id, B.iia_id, A0.hash0)
+B recognizes, that A </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="2"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">reverted </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">to revision A0 (A0.hash0)
+B </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="2"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">removes </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">revision B1 and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="2"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">reverts </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t>to revision B0
+mapped identifiers: B.iia_id (local), A.iia_id (remote)
+last known hashes: B0.hash0, A0.hash0
+approval hashes: B0.hash0, A0.hash0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A sends IIA GET with B.iia_id (remote), receives in response B0 (A.iia_id, B.iia_id, B0.hash0)
+A recognizes, that B </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="2"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">reverted </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t>to revision B0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A changed their mind - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="2"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">removes </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">A1 and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="2"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">reverts </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t>to A0
+mapped identifiers: B.iia_id (local), A.iia_id (remote)
+last known hashes: A0.hash0, B1.hash1
+approval hashes: A1.hash1, B0.hash0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B sends IIA GET, receives in response A0 (A.iia_id, B.iia_id, A0.hash0)
+B recognized that A </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="2"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">reverted </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">to revision A0 (A0.hash0)
+B </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="2"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">removes </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">revision B1 and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="2"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">reverts </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t>to B0
+mapped identifiers: B.iia_id (local), A.iia_id (remote)
+last known hashes: B0.hash0, A0.hash0
+approval hashes: B0.hash0, A1.hash1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A sends IIA GET with B.iia_id (remote), receives in response B0 (A.iia_id, B.iia_id, B0.hash0)
+A recognized, that B </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="2"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t xml:space="preserve">reverted </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t>to revision B0
+mapped identifiers: B.iia_id (local), A.iia_id (remote)
+last known hashes: A0.hash0, B0.hash0
+approval hashes: A1.hash1, B0.hash0</t>
     </r>
   </si>
 </sst>
@@ -2786,8 +2751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2878,7 +2843,7 @@
     </row>
     <row r="15" spans="1:2" ht="126">
       <c r="A15" s="5" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18">
@@ -2893,7 +2858,7 @@
     </row>
     <row r="18" spans="1:2" ht="144">
       <c r="B18" s="5" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18">
@@ -2907,13 +2872,13 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="54">
-      <c r="A21" s="2" t="s">
-        <v>16</v>
+      <c r="A21" s="5" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:2" s="3" customFormat="1" ht="18">
       <c r="A22" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" s="23"/>
     </row>
@@ -2945,8 +2910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2956,7 +2921,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30">
       <c r="A1" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="22"/>
     </row>
@@ -2976,10 +2941,10 @@
     </row>
     <row r="4" spans="1:2" ht="72">
       <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18">
@@ -2990,7 +2955,7 @@
     </row>
     <row r="6" spans="1:2" ht="90">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3"/>
     </row>
@@ -3032,31 +2997,31 @@
     </row>
     <row r="13" spans="1:2" ht="108">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:2" ht="144">
       <c r="A14" s="2"/>
       <c r="B14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:2" ht="108">
       <c r="A16" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:3" ht="90">
-      <c r="A17" s="2" t="s">
-        <v>26</v>
+      <c r="A17" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="B17" s="4"/>
     </row>
@@ -3074,8 +3039,8 @@
     </row>
     <row r="20" spans="1:3" ht="144">
       <c r="A20" s="4"/>
-      <c r="B20" s="2" t="s">
-        <v>27</v>
+      <c r="B20" s="5" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="18">
@@ -3091,42 +3056,42 @@
       <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:3" ht="126">
-      <c r="A23" s="2" t="s">
-        <v>28</v>
+      <c r="A23" s="5" t="s">
+        <v>141</v>
       </c>
       <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:3" ht="216">
       <c r="A24" s="2"/>
       <c r="B24" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C24" s="7"/>
     </row>
     <row r="25" spans="1:3" ht="18">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:3" ht="108">
       <c r="A26" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:3" ht="18">
       <c r="A27" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="23"/>
     </row>
     <row r="28" spans="1:3" ht="72">
       <c r="A28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -3188,7 +3153,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30">
       <c r="A1" s="22" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B1" s="22"/>
     </row>
@@ -3208,10 +3173,10 @@
     </row>
     <row r="4" spans="1:2" ht="72">
       <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18">
@@ -3258,64 +3223,64 @@
     </row>
     <row r="12" spans="1:2" ht="18">
       <c r="A12" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:2" ht="108">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:2" ht="144">
       <c r="A14" s="2"/>
       <c r="B14" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:2" ht="108">
       <c r="A16" s="5" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" ht="180">
       <c r="A17" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" ht="18">
       <c r="A18" s="4"/>
       <c r="B18" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="108">
       <c r="A19" s="4"/>
       <c r="B19" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18">
       <c r="A20" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="23"/>
     </row>
     <row r="21" spans="1:2" ht="72">
       <c r="A21" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -3367,7 +3332,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:B37"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3377,7 +3342,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30">
       <c r="A1" s="22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B1" s="22"/>
     </row>
@@ -3397,10 +3362,10 @@
     </row>
     <row r="4" spans="1:2" ht="72">
       <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18">
@@ -3436,7 +3401,7 @@
     <row r="10" spans="1:2" ht="108">
       <c r="A10" s="4"/>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18">
@@ -3447,19 +3412,19 @@
     </row>
     <row r="12" spans="1:2" ht="18">
       <c r="A12" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:2" ht="108">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:2" ht="108">
       <c r="A14" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B14" s="4"/>
     </row>
@@ -3477,13 +3442,13 @@
     <row r="17" spans="1:2" ht="36">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="108">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18">
@@ -3500,13 +3465,13 @@
     </row>
     <row r="21" spans="1:2" ht="108">
       <c r="A21" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" ht="108">
       <c r="A22" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B22" s="2"/>
     </row>
@@ -3525,13 +3490,13 @@
     <row r="25" spans="1:2" ht="36">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="108">
       <c r="A26" s="8"/>
       <c r="B26" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="18">
@@ -3548,58 +3513,58 @@
     </row>
     <row r="29" spans="1:2" ht="90">
       <c r="A29" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:2" ht="144">
       <c r="A30" s="2"/>
       <c r="B30" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="18">
       <c r="A31" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:2" ht="108">
       <c r="A32" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B32" s="4"/>
     </row>
     <row r="33" spans="1:2" ht="180">
       <c r="A33" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B33" s="4"/>
     </row>
     <row r="34" spans="1:2" ht="18">
       <c r="A34" s="4"/>
       <c r="B34" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="108">
       <c r="A35" s="4"/>
       <c r="B35" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="18">
       <c r="A36" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B36" s="23"/>
     </row>
     <row r="37" spans="1:2" ht="72">
       <c r="A37" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -3629,7 +3594,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30">
       <c r="A1" s="22" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B1" s="22"/>
     </row>
@@ -3649,10 +3614,10 @@
     </row>
     <row r="4" spans="1:2" ht="72">
       <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18">
@@ -3705,31 +3670,31 @@
     </row>
     <row r="13" spans="1:2" ht="108">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:2" ht="144">
       <c r="A14" s="2"/>
       <c r="B14" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:2" ht="108">
       <c r="A16" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" ht="108">
       <c r="A17" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B17" s="4"/>
     </row>
@@ -3748,12 +3713,12 @@
     <row r="20" spans="1:2" ht="36">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="108">
       <c r="B21" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18">
@@ -3770,58 +3735,58 @@
     </row>
     <row r="24" spans="1:2" ht="108">
       <c r="A24" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:2" ht="144">
       <c r="A25" s="2"/>
       <c r="B25" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="18">
       <c r="A26" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:2" ht="108">
       <c r="A27" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B27" s="4"/>
     </row>
     <row r="28" spans="1:2" ht="180">
       <c r="A28" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:2" ht="18">
       <c r="A29" s="8"/>
       <c r="B29" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="108">
       <c r="A30" s="4"/>
       <c r="B30" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="18">
       <c r="A31" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31" s="23"/>
     </row>
     <row r="32" spans="1:2" ht="72">
       <c r="A32" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3851,7 +3816,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30">
       <c r="A1" s="22" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B1" s="22"/>
     </row>
@@ -3871,10 +3836,10 @@
     </row>
     <row r="4" spans="1:2" ht="18">
       <c r="A4" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18">
@@ -3885,7 +3850,7 @@
     </row>
     <row r="6" spans="1:2" ht="90">
       <c r="A6" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B6" s="3"/>
     </row>
@@ -3904,13 +3869,13 @@
     <row r="9" spans="1:2" ht="36">
       <c r="A9" s="4"/>
       <c r="B9" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="111.75" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18">
@@ -3927,50 +3892,50 @@
     </row>
     <row r="13" spans="1:2" ht="108">
       <c r="A13" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:2" ht="144">
       <c r="A14" s="2"/>
       <c r="B14" s="5" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:2" ht="108">
       <c r="A16" s="5" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" ht="72">
       <c r="A17" s="5" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" ht="18">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="144">
       <c r="A19" s="2"/>
       <c r="B19" s="5" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:2" s="4" customFormat="1" ht="162">
       <c r="A20" s="5"/>
       <c r="B20" s="5" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="4" customFormat="1" ht="18">
@@ -3981,40 +3946,40 @@
     </row>
     <row r="22" spans="1:2" s="4" customFormat="1" ht="150" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:2" ht="198">
       <c r="A23" s="5"/>
       <c r="B23" s="20" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18">
       <c r="A24" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="5"/>
     </row>
     <row r="25" spans="1:2" ht="126">
       <c r="A25" s="5" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:2" ht="18">
       <c r="A26" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="23"/>
     </row>
     <row r="27" spans="1:2" ht="54">
       <c r="A27" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -4033,7 +3998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -4046,7 +4011,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30">
       <c r="A1" s="22" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B1" s="22"/>
     </row>
@@ -4066,10 +4031,10 @@
     </row>
     <row r="4" spans="1:3" ht="18">
       <c r="A4" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18">
@@ -4080,7 +4045,7 @@
     </row>
     <row r="6" spans="1:3" ht="90">
       <c r="A6" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="9"/>
@@ -4100,13 +4065,13 @@
     <row r="9" spans="1:3" ht="38.25" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="107.25" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18">
@@ -4123,52 +4088,52 @@
     </row>
     <row r="13" spans="1:3" ht="108">
       <c r="A13" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:3" ht="144">
       <c r="A14" s="2"/>
       <c r="B14" s="5" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:3" ht="108">
       <c r="A16" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:3" ht="72">
       <c r="A17" s="5" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:3" ht="18">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C18" s="8"/>
     </row>
     <row r="19" spans="1:3" ht="90">
       <c r="A19" s="2"/>
       <c r="B19" s="5" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C19" s="10"/>
     </row>
     <row r="20" spans="1:3" s="4" customFormat="1" ht="162">
       <c r="A20" s="5"/>
       <c r="B20" s="5" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C20" s="10"/>
     </row>
@@ -4181,7 +4146,7 @@
     </row>
     <row r="22" spans="1:3" s="4" customFormat="1" ht="72">
       <c r="A22" s="5" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="10"/>
@@ -4189,34 +4154,34 @@
     <row r="23" spans="1:3" ht="198">
       <c r="A23" s="2"/>
       <c r="B23" s="6" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" ht="18">
       <c r="A24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="5"/>
     </row>
     <row r="25" spans="1:3" ht="126">
       <c r="A25" s="11" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:3" ht="18">
       <c r="A26" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="23"/>
     </row>
     <row r="27" spans="1:3" ht="36">
       <c r="A27" s="21" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -4248,79 +4213,79 @@
   <sheetData>
     <row r="1" spans="1:2" ht="27.6" customHeight="1">
       <c r="A1" s="24" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B1" s="24"/>
     </row>
     <row r="2" spans="1:2" s="12" customFormat="1" ht="18">
       <c r="A2" s="23" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B2" s="23"/>
     </row>
     <row r="3" spans="1:2" ht="87.95" customHeight="1">
       <c r="A3" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B3" s="13"/>
     </row>
     <row r="4" spans="1:2" ht="22.7" customHeight="1">
       <c r="A4" s="23" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B4" s="23"/>
     </row>
     <row r="5" spans="1:2" ht="91.5" customHeight="1">
       <c r="A5" s="11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B5" s="11"/>
     </row>
     <row r="6" spans="1:2" ht="297" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="54">
       <c r="A7" s="14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B7" s="11"/>
     </row>
     <row r="8" spans="1:2" s="12" customFormat="1" ht="18">
       <c r="A8" s="23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B8" s="23"/>
     </row>
     <row r="9" spans="1:2" ht="72">
       <c r="A9" s="14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B9" s="11"/>
     </row>
     <row r="10" spans="1:2" ht="72">
       <c r="A10" s="14"/>
       <c r="B10" s="11" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="56.25" customHeight="1">
       <c r="A11" s="14" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B11" s="11"/>
     </row>
     <row r="12" spans="1:2" s="12" customFormat="1" ht="18">
       <c r="A12" s="23" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B12" s="23"/>
     </row>
     <row r="13" spans="1:2" ht="87.95" customHeight="1">
       <c r="A13" s="11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B13" s="11"/>
     </row>
@@ -4334,40 +4299,40 @@
     </row>
     <row r="16" spans="1:2" ht="18">
       <c r="A16" s="23" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B16" s="23"/>
     </row>
     <row r="17" spans="1:2" ht="52.9" customHeight="1">
       <c r="A17" s="11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="288">
       <c r="A18" s="15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="72">
       <c r="A19" s="15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="90">
       <c r="A20" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -4388,8 +4353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4399,7 +4364,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30">
       <c r="A1" s="25" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B1" s="26"/>
     </row>
@@ -4419,10 +4384,10 @@
     </row>
     <row r="4" spans="1:2" ht="72">
       <c r="A4" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18">
@@ -4433,45 +4398,45 @@
     </row>
     <row r="6" spans="1:2" ht="162">
       <c r="A6" s="11" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B6" s="17"/>
     </row>
     <row r="7" spans="1:2" ht="162">
       <c r="A7" s="11" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B7" s="17"/>
     </row>
     <row r="8" spans="1:2" ht="270">
       <c r="A8" s="11"/>
       <c r="B8" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="162">
       <c r="A9" s="11"/>
       <c r="B9" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="4" customFormat="1" ht="18">
       <c r="A10" s="11" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B10" s="11"/>
     </row>
     <row r="11" spans="1:2" s="4" customFormat="1" ht="72">
       <c r="A11" s="11" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="90">
       <c r="A12" s="18" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B12" s="17"/>
     </row>
@@ -4490,19 +4455,19 @@
     <row r="15" spans="1:2" ht="36">
       <c r="A15" s="19"/>
       <c r="B15" s="11" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="108">
       <c r="A16" s="19"/>
       <c r="B16" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="90">
       <c r="A17" s="19"/>
       <c r="B17" s="18" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18">
@@ -4519,13 +4484,13 @@
     </row>
     <row r="20" spans="1:2" ht="36">
       <c r="A20" s="11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B20" s="19"/>
     </row>
     <row r="21" spans="1:2" ht="126">
       <c r="A21" s="11" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="B21" s="19"/>
     </row>
@@ -4544,7 +4509,7 @@
     <row r="24" spans="1:2" ht="144">
       <c r="A24" s="19"/>
       <c r="B24" s="11" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18">
@@ -4561,22 +4526,22 @@
     </row>
     <row r="27" spans="1:2" ht="54">
       <c r="A27" s="11" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="B27" s="19"/>
     </row>
     <row r="28" spans="1:2" ht="18">
       <c r="A28" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="23"/>
     </row>
     <row r="29" spans="1:2" ht="72">
       <c r="A29" s="11" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>